<commit_message>
mock-up of crop data
</commit_message>
<xml_diff>
--- a/Files/crops.xlsx
+++ b/Files/crops.xlsx
@@ -41,9 +41,6 @@
     <t xml:space="preserve">disease</t>
   </si>
   <si>
-    <t xml:space="preserve">av_temperature</t>
-  </si>
-  <si>
     <t xml:space="preserve">av_light</t>
   </si>
   <si>
@@ -53,10 +50,13 @@
     <t xml:space="preserve">yield_mass</t>
   </si>
   <si>
-    <t xml:space="preserve">kak</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/10/2021</t>
+    <t xml:space="preserve">spinach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31/10/2021</t>
   </si>
 </sst>
 </file>
@@ -175,18 +175,17 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="20.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.66"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -217,23 +216,21 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="AMJ1" s="1"/>
+      <c r="AMI1" s="1"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -261,7 +258,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>